<commit_message>
finished ms project file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\km150096\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FAKS\3\USP\projekat\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F125FCEE-19AC-45C9-BECF-EEB7C6FFFAFB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{AD9356FD-91F1-4579-86F4-A239143068A8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="29">
   <si>
     <t>prep</t>
   </si>
@@ -67,16 +66,61 @@
   </si>
   <si>
     <t>tech</t>
+  </si>
+  <si>
+    <t>server sale</t>
+  </si>
+  <si>
+    <t>modemi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">senozri </t>
+  </si>
+  <si>
+    <t>promo materijal</t>
+  </si>
+  <si>
+    <t>2500 po 20</t>
+  </si>
+  <si>
+    <t>2500 po 30</t>
+  </si>
+  <si>
+    <t>senzori</t>
+  </si>
+  <si>
+    <t>staro</t>
+  </si>
+  <si>
+    <t>novo</t>
+  </si>
+  <si>
+    <t>wp8</t>
+  </si>
+  <si>
+    <t>wp9</t>
+  </si>
+  <si>
+    <t>wp10</t>
+  </si>
+  <si>
+    <t>wp11</t>
+  </si>
+  <si>
+    <t>wp12</t>
+  </si>
+  <si>
+    <t>visak</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0_ ;\-#,##0.0\ "/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,8 +140,15 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,6 +163,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,7 +207,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -156,348 +219,14 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="148">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="100">
     <dxf>
       <fill>
         <patternFill>
@@ -1507,19 +1236,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5977A743-B7FB-4D2E-B1FB-27635A180E66}">
-  <dimension ref="A1:M26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A18" sqref="A18"/>
+      <selection pane="topRight" activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1543,7 +1274,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>6</v>
       </c>
@@ -1564,7 +1295,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -1585,7 +1316,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -1606,7 +1337,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1358,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1651,7 +1382,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -1672,7 +1403,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1693,7 +1424,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1714,7 +1445,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -1735,7 +1466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1759,7 +1490,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -1780,7 +1511,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1801,7 +1532,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>8</v>
       </c>
@@ -1822,7 +1553,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>9</v>
       </c>
@@ -1843,7 +1574,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
@@ -1868,7 +1599,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>6</v>
@@ -1891,7 +1622,7 @@
       </c>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>7</v>
@@ -1914,7 +1645,7 @@
       </c>
       <c r="H18" s="3"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>8</v>
@@ -1937,7 +1668,7 @@
       </c>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>9</v>
@@ -1960,7 +1691,7 @@
       </c>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -1987,7 +1718,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>6</v>
       </c>
@@ -2014,7 +1745,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>7</v>
       </c>
@@ -2038,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>8</v>
       </c>
@@ -2059,7 +1790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="18" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -2080,7 +1811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>10</v>
       </c>
@@ -2094,512 +1825,817 @@
         <v>12</v>
       </c>
     </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30">
+        <v>50000</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31">
+        <v>75000</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32">
+        <v>50000</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>16666</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B37" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H37" t="s">
+        <v>21</v>
+      </c>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" t="s">
+        <v>21</v>
+      </c>
+      <c r="K37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6">
+        <v>45</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>100</v>
+      </c>
+      <c r="M38">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6">
+        <v>0</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6">
+        <v>40</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>25</v>
+      </c>
+      <c r="M39">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5">
+        <v>25</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6">
+        <v>0</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>50</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6">
+        <v>60</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6">
+        <v>70</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>22</v>
+      </c>
+      <c r="M41">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5">
+        <v>95</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6">
+        <v>0</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6">
+        <v>20</v>
+      </c>
+      <c r="I42">
+        <v>27</v>
+      </c>
+      <c r="K42">
+        <v>20</v>
+      </c>
+      <c r="M42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B43" s="5">
+        <f>SUM(B38:B42)</f>
+        <v>0</v>
+      </c>
+      <c r="C43" s="5">
+        <f>SUM(C38:C42)</f>
+        <v>120</v>
+      </c>
+      <c r="D43" s="6">
+        <f t="shared" ref="D43:G43" si="1">SUM(D38:D42)</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="6">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="H43">
+        <f t="shared" ref="H43" si="2">SUM(H38:H42)</f>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f t="shared" ref="I43" si="3">SUM(I38:I42)</f>
+        <v>77</v>
+      </c>
+      <c r="J43">
+        <f t="shared" ref="J43" si="4">SUM(J38:J42)</f>
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <f>SUM(K38:K42)</f>
+        <v>167</v>
+      </c>
+      <c r="M43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="G44">
+        <v>91</v>
+      </c>
+      <c r="M44">
+        <f>SUM(M38:M43)</f>
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J46" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="K47">
+        <f>SUM(K43:K46)</f>
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C1">
-    <cfRule type="expression" dxfId="147" priority="124">
+    <cfRule type="expression" dxfId="99" priority="124">
       <formula>ISNUMBER(C1)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="146" priority="123">
+    <cfRule type="expression" dxfId="98" priority="123">
       <formula>ISNUMBER(C6)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="145" priority="122">
+    <cfRule type="expression" dxfId="97" priority="122">
       <formula>ISNUMBER(C11)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="144" priority="121">
+    <cfRule type="expression" dxfId="96" priority="121">
       <formula>ISNUMBER(C16)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="expression" dxfId="143" priority="120">
+    <cfRule type="expression" dxfId="95" priority="120">
       <formula>ISNUMBER(C21)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="142" priority="119">
+    <cfRule type="expression" dxfId="94" priority="119">
       <formula>ISNUMBER(C2)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="141" priority="118">
+    <cfRule type="expression" dxfId="93" priority="118">
       <formula>ISNUMBER(C3)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="140" priority="117">
+    <cfRule type="expression" dxfId="92" priority="117">
       <formula>ISNUMBER(C4)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="139" priority="116">
+    <cfRule type="expression" dxfId="91" priority="116">
       <formula>ISNUMBER(C5)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7">
-    <cfRule type="expression" dxfId="138" priority="115">
+    <cfRule type="expression" dxfId="90" priority="115">
       <formula>ISNUMBER(C7)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="137" priority="114">
+    <cfRule type="expression" dxfId="89" priority="114">
       <formula>ISNUMBER(C8)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="136" priority="113">
+    <cfRule type="expression" dxfId="88" priority="113">
       <formula>ISNUMBER(C9)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="135" priority="112">
+    <cfRule type="expression" dxfId="87" priority="112">
       <formula>ISNUMBER(C10)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="134" priority="111">
+    <cfRule type="expression" dxfId="86" priority="111">
       <formula>ISNUMBER(C12)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="133" priority="110">
+    <cfRule type="expression" dxfId="85" priority="110">
       <formula>ISNUMBER(C13)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="expression" dxfId="132" priority="109">
+    <cfRule type="expression" dxfId="84" priority="109">
       <formula>ISNUMBER(C14)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15">
-    <cfRule type="expression" dxfId="131" priority="108">
+    <cfRule type="expression" dxfId="83" priority="108">
       <formula>ISNUMBER(C15)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="130" priority="107">
+    <cfRule type="expression" dxfId="82" priority="107">
       <formula>ISNUMBER(C17)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="129" priority="106">
+    <cfRule type="expression" dxfId="81" priority="106">
       <formula>ISNUMBER(C18)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="128" priority="105">
+    <cfRule type="expression" dxfId="80" priority="105">
       <formula>ISNUMBER(C19)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="127" priority="104">
+    <cfRule type="expression" dxfId="79" priority="104">
       <formula>ISNUMBER(C20)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22">
-    <cfRule type="expression" dxfId="126" priority="103">
+    <cfRule type="expression" dxfId="78" priority="103">
       <formula>ISNUMBER(C22)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="125" priority="102">
+    <cfRule type="expression" dxfId="77" priority="102">
       <formula>ISNUMBER(C23)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="124" priority="101">
+    <cfRule type="expression" dxfId="76" priority="101">
       <formula>ISNUMBER(C24)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="123" priority="100">
+    <cfRule type="expression" dxfId="75" priority="100">
       <formula>ISNUMBER(C25)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="expression" dxfId="122" priority="1">
+    <cfRule type="expression" dxfId="74" priority="1">
       <formula>ISNUMBER(F25)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="expression" dxfId="74" priority="75">
+    <cfRule type="expression" dxfId="73" priority="75">
       <formula>ISNUMBER(D1)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="73" priority="74">
+    <cfRule type="expression" dxfId="72" priority="74">
       <formula>ISNUMBER(D6)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="72" priority="73">
+    <cfRule type="expression" dxfId="71" priority="73">
       <formula>ISNUMBER(D11)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="expression" dxfId="71" priority="72">
+    <cfRule type="expression" dxfId="70" priority="72">
       <formula>ISNUMBER(D16)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21">
-    <cfRule type="expression" dxfId="70" priority="71">
+    <cfRule type="expression" dxfId="69" priority="71">
       <formula>ISNUMBER(D21)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="69" priority="70">
+    <cfRule type="expression" dxfId="68" priority="70">
       <formula>ISNUMBER(D2)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="68" priority="69">
+    <cfRule type="expression" dxfId="67" priority="69">
       <formula>ISNUMBER(D3)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="67" priority="68">
+    <cfRule type="expression" dxfId="66" priority="68">
       <formula>ISNUMBER(D4)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="66" priority="67">
+    <cfRule type="expression" dxfId="65" priority="67">
       <formula>ISNUMBER(D5)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="65" priority="66">
+    <cfRule type="expression" dxfId="64" priority="66">
       <formula>ISNUMBER(D7)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8">
-    <cfRule type="expression" dxfId="64" priority="65">
+    <cfRule type="expression" dxfId="63" priority="65">
       <formula>ISNUMBER(D8)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="expression" dxfId="63" priority="64">
+    <cfRule type="expression" dxfId="62" priority="64">
       <formula>ISNUMBER(D9)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="62" priority="63">
+    <cfRule type="expression" dxfId="61" priority="63">
       <formula>ISNUMBER(D10)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="61" priority="62">
+    <cfRule type="expression" dxfId="60" priority="62">
       <formula>ISNUMBER(D12)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="expression" dxfId="60" priority="61">
+    <cfRule type="expression" dxfId="59" priority="61">
       <formula>ISNUMBER(D13)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D14">
-    <cfRule type="expression" dxfId="59" priority="60">
+    <cfRule type="expression" dxfId="58" priority="60">
       <formula>ISNUMBER(D14)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="expression" dxfId="58" priority="59">
+    <cfRule type="expression" dxfId="57" priority="59">
       <formula>ISNUMBER(D15)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="expression" dxfId="57" priority="58">
+    <cfRule type="expression" dxfId="56" priority="58">
       <formula>ISNUMBER(D17)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="56" priority="57">
+    <cfRule type="expression" dxfId="55" priority="57">
       <formula>ISNUMBER(D18)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="55" priority="56">
+    <cfRule type="expression" dxfId="54" priority="56">
       <formula>ISNUMBER(D19)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="54" priority="55">
+    <cfRule type="expression" dxfId="53" priority="55">
       <formula>ISNUMBER(D20)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22">
-    <cfRule type="expression" dxfId="53" priority="54">
+    <cfRule type="expression" dxfId="52" priority="54">
       <formula>ISNUMBER(D22)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23">
-    <cfRule type="expression" dxfId="52" priority="53">
+    <cfRule type="expression" dxfId="51" priority="53">
       <formula>ISNUMBER(D23)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24">
-    <cfRule type="expression" dxfId="51" priority="52">
+    <cfRule type="expression" dxfId="50" priority="52">
       <formula>ISNUMBER(D24)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="expression" dxfId="50" priority="51">
+    <cfRule type="expression" dxfId="49" priority="51">
       <formula>ISNUMBER(D25)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="expression" dxfId="49" priority="50">
+    <cfRule type="expression" dxfId="48" priority="50">
       <formula>ISNUMBER(E1)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="48" priority="49">
+    <cfRule type="expression" dxfId="47" priority="49">
       <formula>ISNUMBER(E6)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="expression" dxfId="47" priority="48">
+    <cfRule type="expression" dxfId="46" priority="48">
       <formula>ISNUMBER(E11)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="expression" dxfId="46" priority="47">
+    <cfRule type="expression" dxfId="45" priority="47">
       <formula>ISNUMBER(E16)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="expression" dxfId="45" priority="46">
+    <cfRule type="expression" dxfId="44" priority="46">
       <formula>ISNUMBER(E21)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="44" priority="45">
+    <cfRule type="expression" dxfId="43" priority="45">
       <formula>ISNUMBER(E2)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="43" priority="44">
+    <cfRule type="expression" dxfId="42" priority="44">
       <formula>ISNUMBER(E3)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="42" priority="43">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>ISNUMBER(E4)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="41" priority="42">
+    <cfRule type="expression" dxfId="40" priority="42">
       <formula>ISNUMBER(E5)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="expression" dxfId="40" priority="41">
+    <cfRule type="expression" dxfId="39" priority="41">
       <formula>ISNUMBER(E7)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="38" priority="40">
       <formula>ISNUMBER(E8)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="37" priority="39">
       <formula>ISNUMBER(E9)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="37" priority="38">
+    <cfRule type="expression" dxfId="36" priority="38">
       <formula>ISNUMBER(E10)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="35" priority="37">
       <formula>ISNUMBER(E12)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="34" priority="36">
       <formula>ISNUMBER(E13)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="33" priority="35">
       <formula>ISNUMBER(E14)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="32" priority="34">
       <formula>ISNUMBER(E15)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E17">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="31" priority="33">
       <formula>ISNUMBER(E17)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="31" priority="32">
+    <cfRule type="expression" dxfId="30" priority="32">
       <formula>ISNUMBER(E18)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="expression" dxfId="30" priority="31">
+    <cfRule type="expression" dxfId="29" priority="31">
       <formula>ISNUMBER(E19)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="29" priority="30">
+    <cfRule type="expression" dxfId="28" priority="30">
       <formula>ISNUMBER(E20)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="28" priority="29">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>ISNUMBER(E22)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="expression" dxfId="27" priority="28">
+    <cfRule type="expression" dxfId="26" priority="28">
       <formula>ISNUMBER(E23)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="26" priority="27">
+    <cfRule type="expression" dxfId="25" priority="27">
       <formula>ISNUMBER(E24)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="expression" dxfId="25" priority="26">
+    <cfRule type="expression" dxfId="24" priority="26">
       <formula>ISNUMBER(E25)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="23" priority="25">
       <formula>ISNUMBER(F1)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="expression" dxfId="23" priority="24">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>ISNUMBER(F6)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F11">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="21" priority="23">
       <formula>ISNUMBER(F11)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16">
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>ISNUMBER(F16)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F21">
-    <cfRule type="expression" dxfId="20" priority="21">
+    <cfRule type="expression" dxfId="19" priority="21">
       <formula>ISNUMBER(F21)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2">
-    <cfRule type="expression" dxfId="19" priority="20">
+    <cfRule type="expression" dxfId="18" priority="20">
       <formula>ISNUMBER(F2)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>ISNUMBER(F3)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="expression" dxfId="17" priority="18">
+    <cfRule type="expression" dxfId="16" priority="18">
       <formula>ISNUMBER(F4)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="15" priority="17">
       <formula>ISNUMBER(F5)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F7">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>ISNUMBER(F7)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="expression" dxfId="14" priority="15">
+    <cfRule type="expression" dxfId="13" priority="15">
       <formula>ISNUMBER(F8)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F9">
-    <cfRule type="expression" dxfId="13" priority="14">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>ISNUMBER(F9)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>ISNUMBER(F10)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F12">
-    <cfRule type="expression" dxfId="11" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>ISNUMBER(F12)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F13">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="9" priority="11">
       <formula>ISNUMBER(F13)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F14">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>ISNUMBER(F14)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="7" priority="9">
       <formula>ISNUMBER(F15)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F17">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>ISNUMBER(F17)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>ISNUMBER(F18)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>ISNUMBER(F19)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>ISNUMBER(F20)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>ISNUMBER(F22)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F23">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>ISNUMBER(F23)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>ISNUMBER(F24)=FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Format error (1 decimal only)" prompt="Please encode number of days - 1 decimal only" sqref="C1:F25" xr:uid="{03B9FFC7-343D-4372-AD2D-8F1A8CA83003}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Format error (1 decimal only)" prompt="Please encode number of days - 1 decimal only" sqref="C1:F25">
       <formula1>C1=INT(C1*10)/10</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>